<commit_message>
Completed Associated Relation with User Product Cart
</commit_message>
<xml_diff>
--- a/controllers/Product.xlsx
+++ b/controllers/Product.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="15">
   <si>
     <t>ID</t>
   </si>
@@ -28,34 +28,34 @@
     <t>Category</t>
   </si>
   <si>
+    <t>Xiaoni</t>
+  </si>
+  <si>
+    <t>5000/uploads/Hating Game.png</t>
+  </si>
+  <si>
     <t>Nokia</t>
   </si>
   <si>
-    <t>5000/uploads/Hating Game.png</t>
+    <t>New Data</t>
+  </si>
+  <si>
+    <t>http://localhost:5000/uploads/Emotion Machine.png</t>
   </si>
   <si>
     <t>Samsung</t>
   </si>
   <si>
-    <t>Xiaoni</t>
+    <t>Fault</t>
+  </si>
+  <si>
+    <t>http://localhost:5000/uploads/Fault.png</t>
   </si>
   <si>
     <t>Huwaei</t>
   </si>
   <si>
     <t>http://localhost:5000//uploads/FasterFene.png</t>
-  </si>
-  <si>
-    <t>Fault</t>
-  </si>
-  <si>
-    <t>http://localhost:5000/uploads/Fault.png</t>
-  </si>
-  <si>
-    <t>New Data</t>
-  </si>
-  <si>
-    <t>http://localhost:5000/uploads/Emotion Machine.png</t>
   </si>
 </sst>
 </file>
@@ -436,7 +436,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E15"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="3" width="20" customWidth="1"/>
@@ -463,7 +463,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -480,7 +480,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
@@ -492,21 +492,21 @@
         <v>6</v>
       </c>
       <c r="E3">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
       <c r="C4">
-        <v>1200</v>
+        <v>4000</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E4">
         <v>5</v>
@@ -514,10 +514,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C5">
         <v>1200</v>
@@ -531,10 +531,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C6">
         <v>1200</v>
@@ -551,7 +551,7 @@
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C7">
         <v>1200</v>
@@ -565,10 +565,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C8">
         <v>1200</v>
@@ -582,10 +582,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C9">
         <v>1200</v>
@@ -599,10 +599,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C10">
         <v>1200</v>
@@ -611,36 +611,33 @@
         <v>6</v>
       </c>
       <c r="E10">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C11">
-        <v>1700</v>
+        <v>1200</v>
       </c>
       <c r="D11" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E11">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
       </c>
-      <c r="C12">
-        <v>1700</v>
-      </c>
       <c r="D12" t="s">
         <v>12</v>
       </c>
@@ -650,19 +647,53 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13">
+        <v>1700</v>
+      </c>
+      <c r="D13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>21</v>
+      </c>
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14">
+        <v>1700</v>
+      </c>
+      <c r="D14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>20</v>
+      </c>
+      <c r="B15" t="s">
         <v>13</v>
       </c>
-      <c r="C13">
-        <v>4000</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="C15">
+        <v>1700</v>
+      </c>
+      <c r="D15" t="s">
         <v>14</v>
       </c>
-      <c r="E13">
-        <v>5</v>
+      <c r="E15">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>